<commit_message>
upgread frame support webgl
</commit_message>
<xml_diff>
--- a/Assets/island/DBCfg/DataCfg.xlsx
+++ b/Assets/island/DBCfg/DataCfg.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25500" windowHeight="15600" tabRatio="827" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15600" tabRatio="827"/>
   </bookViews>
   <sheets>
     <sheet name="配置表cfg" sheetId="1" r:id="rId1"/>
@@ -10548,11 +10548,11 @@
   </sheetPr>
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomRight" activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -10770,7 +10770,7 @@
         <v>1</v>
       </c>
       <c r="L7" s="2">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -10917,7 +10917,7 @@
   </sheetPr>
   <dimension ref="A1:BM45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane xSplit="5" ySplit="6" topLeftCell="F26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>

</xml_diff>